<commit_message>
finalizando tarefa de vacinas FPOO
</commit_message>
<xml_diff>
--- a/FPOO/Java/aula2_verde/workspace/Vacinas/excel/vacinas.xlsx
+++ b/FPOO/Java/aula2_verde/workspace/Vacinas/excel/vacinas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25822"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/645ba0ac008cf914/Área de Trabalho/SENAI/Diretorios/desenvolvimento-de-sistemas/FPOO/Java/aula2_verde/workspace/Vacinas/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desenvolvimento-de-sistemas\FPOO\Java\aula2_verde\workspace\Vacinas\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{04D295F4-0C26-4D8F-8219-D137E466BB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28092491-1DB7-4D8C-A4A1-ADF4F4979BC0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF7D15E-0D9C-4949-992B-3513122F914D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5711CB8F-A48F-49F1-984E-5C46A9A740EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5711CB8F-A48F-49F1-984E-5C46A9A740EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>Nome do Pet</t>
   </si>
@@ -207,12 +199,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -230,6 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,9 +537,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742A3320-24AC-4CB0-82FC-D9E16B036AEA}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:E6"/>
     </sheetView>
   </sheetViews>
@@ -557,9 +550,11 @@
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -568,7 +563,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -585,7 +580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -617,7 +612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -653,7 +648,7 @@
         <v>44865</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -670,7 +665,7 @@
         <v>44864</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -687,7 +682,7 @@
         <v>44865</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
@@ -696,7 +691,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -713,7 +708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -730,7 +725,21 @@
         <v>44783</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="10">
+        <v>44862</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -738,8 +747,20 @@
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="10">
+        <v>44864</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -756,24 +777,24 @@
         <v>44862</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3">
-        <v>44864</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>44783</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2</v>
       </c>

</xml_diff>